<commit_message>
fixed issue#166 - wrong target cell data list positions
</commit_message>
<xml_diff>
--- a/jxls-examples/src/main/resources/org/jxls/demo/issue/issue166_template.xlsx
+++ b/jxls-examples/src/main/resources/org/jxls/demo/issue/issue166_template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\git-repos\jxls2-eclipse-2019-03\jxls-examples\src\main\resources\org\jxls\demo\issue\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A09B798-E016-494E-8EFB-B10BD11A1EAD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="1110" windowWidth="23445" windowHeight="13155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1845" yWindow="1110" windowWidth="23445" windowHeight="13155"/>
   </bookViews>
   <sheets>
     <sheet name="Tab1" sheetId="1" r:id="rId1"/>
@@ -31,19 +25,20 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Welly Hong</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>jx:area(lastCell="B4")
 jx:each(items="rs0" var="rec" lastCell="B2")</t>
@@ -55,19 +50,20 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Welly Hong</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A2" authorId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="204"/>
           </rPr>
           <t>jx:area(lastCell="B4")
 jx:each(items="rs0" var="xec" lastCell="B2")</t>
@@ -102,7 +98,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -129,7 +125,8 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="4">
@@ -173,9 +170,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Gut" xfId="1" builtinId="26"/>
-    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="2" builtinId="27"/>
+    <cellStyle name="Хороший" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -479,37 +476,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="23" max="23" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.1328125" customWidth="1"/>
+    <col min="23" max="23" width="15.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -518,7 +513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -535,7 +530,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
       <c r="W12" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,29 +543,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -579,7 +574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>

</xml_diff>